<commit_message>
add html and update xlsx
</commit_message>
<xml_diff>
--- a/indices.xlsx
+++ b/indices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kyo\Documents\projects\check-my-exercises\check-my-workouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CB8CB0-938D-4E46-849D-4918D8EA7137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5C621A-9A15-43F2-91FE-890F3B704B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28860" yWindow="-15" windowWidth="28920" windowHeight="15720" xr2:uid="{C4DA5354-F5DE-44B1-8E56-AD3A94FA23EF}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{C4DA5354-F5DE-44B1-8E56-AD3A94FA23EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Homme" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="11">
   <si>
     <t>Categorie</t>
   </si>
@@ -52,6 +52,24 @@
   </si>
   <si>
     <t>push genou</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -104,6 +122,50 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{75C8FFF1-9C42-415D-9C01-4E95C637FD88}" name="Table1" displayName="Table1" ref="A1:H5" totalsRowShown="0">
+  <autoFilter ref="A1:H5" xr:uid="{75C8FFF1-9C42-415D-9C01-4E95C637FD88}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H5">
+    <sortCondition ref="A2:A5"/>
+    <sortCondition ref="B2:B5"/>
+    <sortCondition ref="C2:C5"/>
+  </sortState>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{32ABE7E1-7C18-4570-A4BC-F755E780EF0A}" name="Categorie"/>
+    <tableColumn id="2" xr3:uid="{95799582-89B5-4562-81BE-2481EAA953F9}" name="Exercice"/>
+    <tableColumn id="3" xr3:uid="{EE8B039F-C1CB-4489-B86E-A61B06C08AD1}" name="Age"/>
+    <tableColumn id="4" xr3:uid="{4BBF04D7-6B34-4F8D-B13E-C54F7F3DE410}" name="1"/>
+    <tableColumn id="5" xr3:uid="{95008E09-EB8E-4584-AFB1-7176795BAFCB}" name="2"/>
+    <tableColumn id="6" xr3:uid="{DA3C7176-3EFA-4467-B28D-337FB6EC6033}" name="3"/>
+    <tableColumn id="7" xr3:uid="{01FB79B2-9BD2-4DC8-AE07-0FE7709F3BFE}" name="4"/>
+    <tableColumn id="8" xr3:uid="{DAAA5BE7-509A-4923-8D8B-1C581EC77EC2}" name="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E8E7D1F0-41F0-46AD-A6B9-5091AC326F0F}" name="Table13" displayName="Table13" ref="A1:H5" totalsRowShown="0">
+  <autoFilter ref="A1:H5" xr:uid="{E8E7D1F0-41F0-46AD-A6B9-5091AC326F0F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H5">
+    <sortCondition ref="A4294967285:A4294967288"/>
+    <sortCondition ref="B4294967285:B4294967288"/>
+    <sortCondition ref="C4294967285:C4294967288"/>
+  </sortState>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{46FE9209-B922-4E7A-AF6A-65B3E7757877}" name="Categorie"/>
+    <tableColumn id="2" xr3:uid="{02E3EDB4-7E65-4916-B04C-D82A291C2037}" name="Exercice"/>
+    <tableColumn id="3" xr3:uid="{CF48295F-7DC7-4BF1-9DBF-AC52A8EC201E}" name="Age"/>
+    <tableColumn id="4" xr3:uid="{97813AE0-62C9-4169-B746-AF8F5C22F5F2}" name="1"/>
+    <tableColumn id="5" xr3:uid="{27B3DDBB-713A-4770-BD89-78718AD800EE}" name="2"/>
+    <tableColumn id="6" xr3:uid="{ADCFECC4-0E6C-4BA7-BB45-6B830CB58DF1}" name="3"/>
+    <tableColumn id="7" xr3:uid="{9C5E7419-4969-4157-938C-713475CF016D}" name="4"/>
+    <tableColumn id="8" xr3:uid="{98AF793F-3079-49BF-908B-787BB2800416}" name="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -423,182 +485,300 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB5384B-5AB8-4DD9-8669-549EC42B0826}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>40</v>
+      </c>
+      <c r="G2">
+        <v>60</v>
+      </c>
+      <c r="H2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <v>40</v>
+      </c>
+      <c r="G3">
+        <v>60</v>
+      </c>
+      <c r="H3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="C4">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>21</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+      <c r="H4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="C5">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <v>17</v>
       </c>
-      <c r="C4">
+      <c r="F5">
+        <v>21</v>
+      </c>
+      <c r="G5">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>21</v>
-      </c>
-      <c r="C5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>30</v>
-      </c>
-      <c r="C6">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
+      <c r="H5">
         <v>39</v>
-      </c>
-      <c r="C7">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8ADC812-6DB3-48DD-9BC8-5925A8923BC5}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>21</v>
+      </c>
+      <c r="G2">
+        <v>30</v>
+      </c>
+      <c r="H2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>17</v>
+      </c>
+      <c r="F3">
+        <v>21</v>
+      </c>
+      <c r="G3">
+        <v>30</v>
+      </c>
+      <c r="H3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="C4">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>40</v>
+      </c>
+      <c r="G4">
+        <v>60</v>
+      </c>
+      <c r="H4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>17</v>
-      </c>
-      <c r="C4">
+      <c r="C5">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>21</v>
-      </c>
-      <c r="C5">
+      <c r="F5">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>30</v>
-      </c>
-      <c r="C6">
+      <c r="G5">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>39</v>
-      </c>
-      <c r="C7">
+      <c r="H5">
         <v>80</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>